<commit_message>
debug tounament and update result
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Projects/CSE240A/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yux\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EFB1D9-DA36-CD44-9EED-C4C85CBEAE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC5E71B-E734-4601-9EB4-6007C67CA887}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="500" windowWidth="34260" windowHeight="28300" xr2:uid="{9C3B5EE5-76C3-DB4F-8A59-D01E0CDCA4C8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11805" xr2:uid="{9C3B5EE5-76C3-DB4F-8A59-D01E0CDCA4C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -75,12 +64,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -108,7 +104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,7 +122,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -144,7 +140,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -157,8 +153,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Performance of branch predictor (%misprediction rate)</a:t>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Performance of different branch predictors </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -176,7 +172,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -188,13 +184,23 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4680755579127723E-2"/>
+          <c:y val="9.2296040798775653E-2"/>
+          <c:w val="0.88606057562852469"/>
+          <c:h val="0.75080363046222265"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -229,22 +235,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>mm_2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mm_1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int_2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>int_1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>int_2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>fp_2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>fp_1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>fp_2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>mm_1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>mm_2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -256,22 +262,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17.57</c:v>
+                  <c:v>8.4830000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78</c:v>
+                  <c:v>2.581</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.145</c:v>
+                  <c:v>0.42599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.577</c:v>
+                  <c:v>12.622</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.275</c:v>
+                  <c:v>3.246</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.75</c:v>
+                  <c:v>0.99099999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -312,22 +318,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>mm_2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mm_1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int_2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>int_1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>int_2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>fp_2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>fp_1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>fp_2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>mm_1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>mm_2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -339,22 +345,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>13.9</c:v>
+                  <c:v>10.138</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42599999999999999</c:v>
+                  <c:v>6.6959999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84199999999999997</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>13.839</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.5</c:v>
+                  <c:v>1.6779999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.228999999999999</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -395,22 +401,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>mm_2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mm_1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int_2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>int_1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>int_2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>fp_2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>fp_1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>fp_2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>mm_1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>mm_2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -422,22 +428,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.808</c:v>
+                  <c:v>6.7519999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28199999999999997</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81499999999999995</c:v>
+                  <c:v>0.27600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1459999999999999</c:v>
+                  <c:v>10.753</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94799999999999995</c:v>
+                  <c:v>1.327</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.8120000000000003</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,22 +484,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>mm_2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mm_1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int_2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>int_1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>int_2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>fp_2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>fp_1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>fp_2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>mm_1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>mm_2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -505,22 +511,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.803000000000001</c:v>
+                  <c:v>6.6539999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28399999999999997</c:v>
+                  <c:v>1.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81399999999999995</c:v>
+                  <c:v>0.27900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.222</c:v>
+                  <c:v>10.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0089999999999999</c:v>
+                  <c:v>0.219</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6920000000000002</c:v>
+                  <c:v>0.81100000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,22 +567,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>mm_2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mm_1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int_2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>int_1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>int_2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>fp_2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>fp_1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>fp_2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>mm_1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>mm_2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -588,22 +594,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>11.446999999999999</c:v>
+                  <c:v>6.9349999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>1.0029999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81499999999999995</c:v>
+                  <c:v>0.27500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1459999999999999</c:v>
+                  <c:v>11.407999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97199999999999998</c:v>
+                  <c:v>1.327</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9889999999999999</c:v>
+                  <c:v>0.81200000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,8 +639,72 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Trace</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.2485494549617662E-3"/>
+              <c:y val="0.39803310300498151"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -655,7 +725,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -667,7 +737,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1113007215"/>
@@ -698,8 +768,72 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Misprediction Rate (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44594073134008455"/>
+              <c:y val="0.895084900101773"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -714,7 +848,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -726,7 +860,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1113485919"/>
@@ -756,7 +890,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -768,7 +902,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -796,15 +930,15 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200" baseline="0"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1359,15 +1493,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:colOff>444499</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1396,7 +1530,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1695,15 +1829,16 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1729,144 +1864,146 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>17.57</v>
+        <v>8.4830000000000005</v>
       </c>
       <c r="C2">
-        <v>13.9</v>
+        <v>10.138</v>
       </c>
       <c r="D2">
-        <v>10.808</v>
+        <v>6.7519999999999998</v>
       </c>
       <c r="E2">
-        <v>10.803000000000001</v>
+        <v>6.6539999999999999</v>
       </c>
       <c r="F2">
-        <v>11.446999999999999</v>
+        <v>6.9349999999999996</v>
       </c>
       <c r="H2">
         <f>(I1*POWER(2,J1)+2*POWER(2,I1))/1024</f>
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>0.78</v>
+        <v>2.581</v>
       </c>
       <c r="C3">
-        <v>0.42599999999999999</v>
+        <v>6.6959999999999997</v>
       </c>
       <c r="D3">
-        <v>0.28199999999999997</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.28399999999999997</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="F3">
-        <v>0.28000000000000003</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H3">
         <f>2*POWER(2,H1)/1024</f>
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1.145</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="C4">
-        <v>0.84199999999999997</v>
+        <v>0.42</v>
       </c>
       <c r="D4">
-        <v>0.81499999999999995</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="E4">
-        <v>0.81399999999999995</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="F4">
-        <v>0.81499999999999995</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="H4">
         <f>2*POWER(2,J1)/1024</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>7.577</v>
+        <v>12.622</v>
       </c>
       <c r="C5">
-        <v>1.5</v>
+        <v>13.839</v>
       </c>
       <c r="D5">
-        <v>1.1459999999999999</v>
+        <v>10.753</v>
       </c>
       <c r="E5">
-        <v>0.222</v>
+        <v>10.77</v>
       </c>
       <c r="F5">
-        <v>1.1459999999999999</v>
+        <v>11.407999999999999</v>
       </c>
       <c r="H5">
         <f>SUM(H2:H4)</f>
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>10.275</v>
+        <v>3.246</v>
       </c>
       <c r="C6">
-        <v>6.5</v>
+        <v>1.6779999999999999</v>
       </c>
       <c r="D6">
-        <v>0.94799999999999995</v>
+        <v>1.327</v>
       </c>
       <c r="E6">
-        <v>1.0089999999999999</v>
+        <v>0.219</v>
       </c>
       <c r="F6">
-        <v>0.97199999999999998</v>
+        <v>1.327</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>12.75</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="C7">
-        <v>10.228999999999999</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="D7">
-        <v>6.8120000000000003</v>
+        <v>0.81</v>
       </c>
       <c r="E7">
-        <v>6.6920000000000002</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="F7">
-        <v>6.9889999999999999</v>
+        <v>0.81200000000000006</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>